<commit_message>
fix: all scripts, test cases, and checklist are now ready
</commit_message>
<xml_diff>
--- a/exam details/Test Cases.xlsx
+++ b/exam details/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMMING_HABIT\automation-exam\exam details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0AB197-0EB8-4E2C-A19D-09ECCE5D9470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C087B-2C51-45C8-92BA-229E74D7180C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="206">
   <si>
     <t>Application name</t>
   </si>
@@ -100,120 +100,7 @@
 correct username and password</t>
   </si>
   <si>
-    <t>1. Go to https://www.saucedemo.com/
-2. Enter a valid username (standard_user)
-3. Enter a valid password (secrect_sauce)
-4. Click the Login button</t>
-  </si>
-  <si>
     <t>CLOSED</t>
-  </si>
-  <si>
-    <r>
-      <t>1. Go to https://www.saucedemo.com/
-2. Enter a valid username (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>stand@rd_us3r</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-3. Enter a valid password (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>secr3ct_saUce</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-4. Click the Login button</t>
-    </r>
-  </si>
-  <si>
-    <t>Software Testing - Swag Labs</t>
-  </si>
-  <si>
-    <r>
-      <t>1. Go to https://www.saucedemo.com/
-2. Enter a valid username (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>stand@rd_us3r</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-3. Enter a valid password (secrect_sauce)
-4. Click the Login button</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1. Go to https://www.saucedemo.com/
-2. Enter a valid username (standard_user)
-3. Enter a valid password (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>secr3ct_saUce</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-4. Click the Login button</t>
-    </r>
   </si>
   <si>
     <r>
@@ -419,12 +306,6 @@
 4. Click the Login button</t>
   </si>
   <si>
-    <t>1. Go to https://www.saucedemo.com/
-2. Leave the username empty
-3. Enter a password (secrect_sauce)
-4. Click the Login button</t>
-  </si>
-  <si>
     <t>Login procedures</t>
   </si>
   <si>
@@ -504,9 +385,6 @@
   </si>
   <si>
     <t>User should be able to redirect to inventory e-commerce and see all products below.</t>
-  </si>
-  <si>
-    <t>User should see the cart icon if incrementing to one</t>
   </si>
   <si>
     <t>User see the cart icon incremented to one</t>
@@ -630,9 +508,6 @@
     <t>ENHANCEMENT</t>
   </si>
   <si>
-    <t>The user can reset the 'Add to cart' number but cannot reset the button label from 'Remove' back to 'Add to cart,' and the sorting does not revert to the default setting.</t>
-  </si>
-  <si>
     <t>Please see the screenshot id 5</t>
   </si>
   <si>
@@ -858,17 +733,6 @@
       </rPr>
       <t>", stay in the checkout information page, and should not move forward to the next step of checkout.</t>
     </r>
-  </si>
-  <si>
-    <t>1. Go to https://www.saucedemo.com/
-2. Enter a valid username (standard_user)
-3. Enter a valid password (secrect_sauce)
-4. Click the Login button
-5. Click add to cart button on chosen product/s
-6. Click the cart icon
-7. Click the checkout button
-8. Fill-in first name, last name, and zip code information
-9. Click continue</t>
   </si>
   <si>
     <t>User should redirect to checkout overview page where the quantity and description of product/s, payment information, shipping information, and price total are all presented.</t>
@@ -1612,6 +1476,165 @@
   </si>
   <si>
     <t>Continue button is higher than the average place</t>
+  </si>
+  <si>
+    <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (standard_user)
+3. Enter a valid password (secret_sauce)
+4. Click the Login button</t>
+  </si>
+  <si>
+    <t>1. Go to https://www.saucedemo.com/
+2. Leave the username empty
+3. Enter a password (secret_sauce)
+4. Click the Login button</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strandard_users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+3. Enter a valid password (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sentret_sows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+4. Click the Login button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strandard_users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+3. Enter a valid password (secret_sauce)
+4. Click the Login button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (standard_user)
+3. Enter a valid password (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sentret_sows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+4. Click the Login button</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The user can reset the 'Add to cart' number but cannot reset the button label from 'Remove' back to 'Add to cart,' and the sorting does not revert to the default setting. </t>
+  </si>
+  <si>
+    <t>Test Finding Results - Swag Labs</t>
+  </si>
+  <si>
+    <t>User should see the cart icon incrementing to one per click on add to cart button</t>
+  </si>
+  <si>
+    <t>Verify if user is able to checkout with product/s on its cart</t>
+  </si>
+  <si>
+    <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (standard_user)
+3. Enter a valid password (secrect_sauce)
+4. Click the Login button
+5. Once redirects to inventory e-commerce
+6. Click add to cart button on chosen product/s
+7. Click the cart icon
+8. Redirects to cart page
+9. Click checkout button
+10. Fill in information
+11. Click continue</t>
+  </si>
+  <si>
+    <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (standard_user)
+3. Enter a valid password (secrect_sauce)
+4. Click the Login button
+5. Click add to cart button on chosen product/s
+6. Click the cart icon
+7. Click the checkout button
+8. Fill-in first name, last name, and zip code information
+9. Click continue
+10. Click finish</t>
+  </si>
+  <si>
+    <t>User should be able to checkout product/s that are added to cart, fill-in informaton, and finish the process of transaction.</t>
+  </si>
+  <si>
+    <t>User is able to checkout product/s, fill-in information, and finish the process of transaction.</t>
   </si>
 </sst>
 </file>
@@ -1857,6 +1880,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1864,6 +1899,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1879,21 +1917,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2728,477 +2751,470 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
+      <c r="A1" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
     </row>
     <row r="5" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
     </row>
     <row r="8" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
     </row>
     <row r="9" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
     </row>
     <row r="11" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
-      <c r="K14" s="15" t="s">
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="K14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="17"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="21"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="25"/>
-      <c r="K15" s="27" t="s">
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="K15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="17"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="21"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="25"/>
-      <c r="K16" s="18" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="K16" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="20"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="25"/>
     </row>
     <row r="19" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="25"/>
-      <c r="K19" s="15" t="s">
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="K19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="17"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="21"/>
     </row>
     <row r="20" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="25"/>
-      <c r="K20" s="15" t="s">
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="K20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="17"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="21"/>
     </row>
     <row r="21" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="25"/>
-      <c r="K21" s="18" t="s">
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="K21" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="20"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="25"/>
     </row>
     <row r="24" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="24"/>
-      <c r="I24" s="25"/>
-      <c r="K24" s="21">
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
+      <c r="K24" s="26">
         <v>45433</v>
       </c>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-      <c r="V24" s="22"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:Z11"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="K14:V14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K15:V15"/>
-    <mergeCell ref="K16:V16"/>
     <mergeCell ref="K19:V19"/>
     <mergeCell ref="K20:V20"/>
     <mergeCell ref="K21:V21"/>
@@ -3207,6 +3223,13 @@
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A1:Z11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="K14:V14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="K15:V15"/>
+    <mergeCell ref="K16:V16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K15" r:id="rId1" xr:uid="{B39E7FA7-0077-4592-BE7E-C6FE950055E9}"/>
@@ -3220,7 +3243,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3238,19 +3261,19 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3258,16 +3281,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -3278,10 +3301,10 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -3290,14 +3313,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -3307,13 +3330,13 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -3322,16 +3345,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -3340,16 +3363,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -3358,19 +3381,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3380,10 +3403,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C1E1C6-748F-4782-83CA-6948B67C52D3}">
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3426,7 +3449,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -3444,16 +3467,16 @@
         <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>19</v>
@@ -3465,19 +3488,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>19</v>
@@ -3489,19 +3512,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>196</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>19</v>
@@ -3513,19 +3536,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>197</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>19</v>
@@ -3537,19 +3560,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>19</v>
@@ -3561,19 +3584,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>19</v>
@@ -3585,19 +3608,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
+        <v>194</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
@@ -3609,19 +3632,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>19</v>
@@ -3633,19 +3656,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
@@ -3657,19 +3680,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>19</v>
@@ -3681,19 +3704,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>19</v>
@@ -3705,19 +3728,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>19</v>
@@ -3729,30 +3752,30 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -3767,25 +3790,25 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3793,25 +3816,25 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3819,25 +3842,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3845,25 +3868,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3871,25 +3894,25 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="H21" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3897,25 +3920,25 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3923,22 +3946,22 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H23" s="3"/>
     </row>
@@ -3947,30 +3970,30 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -3985,19 +4008,19 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>56</v>
+        <v>200</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>19</v>
@@ -4009,19 +4032,19 @@
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>19</v>
@@ -4030,7 +4053,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -4045,432 +4068,446 @@
         <v>24</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>25</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>80</v>
+        <v>204</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>84</v>
+        <v>205</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G38" s="5"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G39" s="5"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
+        <v>35</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="5"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
         <v>36</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="B42" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>37</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="B43" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
         <v>38</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>39</v>
-      </c>
       <c r="B45" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G45" s="5"/>
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
+        <v>40</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
         <v>41</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="3"/>
+      <c r="B48" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -5232,6 +5269,16 @@
       <c r="G124" s="5"/>
       <c r="H124" s="3"/>
     </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="3"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A16:H16"/>
@@ -5240,7 +5287,7 @@
     <mergeCell ref="A28:H28"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G26:G27 G44:G124 G4:G15 G17:G24 G29:G42" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G45:G125 G4:G15 G17:G24 G26:G27 G29:G43" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
       <formula1>"A- High, B - Medium, C - Low, None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3" xr:uid="{9E7A5853-1C00-445C-9290-798981E423AE}">
@@ -5255,8 +5302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9830D0D6-2CFD-44B9-BA8F-41E0191DF7BC}">
   <dimension ref="A1:B591"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="L115" sqref="L115"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="L135" sqref="L135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5270,7 +5317,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="307.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: update checklist and test cases before the assessment
</commit_message>
<xml_diff>
--- a/exam details/Test Cases.xlsx
+++ b/exam details/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMMING_HABIT\automation-exam\exam details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C087B-2C51-45C8-92BA-229E74D7180C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC7199-7832-418E-BA82-3941CE91F6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="214">
   <si>
     <t>Application name</t>
   </si>
@@ -1635,6 +1635,42 @@
   </si>
   <si>
     <t>User is able to checkout product/s, fill-in information, and finish the process of transaction.</t>
+  </si>
+  <si>
+    <t>Verify if the specific product is the same after clicking the title</t>
+  </si>
+  <si>
+    <t>Verify if add to cart and remove button are working on a specific product and verify the cart badge if incrementing or decrementing</t>
+  </si>
+  <si>
+    <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (standard_user)
+3. Enter a valid password (secrect_sauce)
+4. Click the Login button
+5. Once redirects to inventory e-commerce
+6. Click any product title</t>
+  </si>
+  <si>
+    <t>1. Go to https://www.saucedemo.com/
+2. Enter a valid username (standard_user)
+3. Enter a valid password (secrect_sauce)
+4. Click the Login button
+5. Once redirects to inventory e-commerce
+6. Click any product title
+7. Click the 'add to cart' button
+8. Click the 'remove' button</t>
+  </si>
+  <si>
+    <t>The user able to add to cart and remove product, also able to see the cart badge incrementing and decrementing accordingly.</t>
+  </si>
+  <si>
+    <t>The user should be able to click the 'add to cart' and check the cart icon if incremented and able to click the 'remove' button and check the cart icon if decremented.</t>
+  </si>
+  <si>
+    <t>The user should be able to see the same title of the clicked product.</t>
+  </si>
+  <si>
+    <t>The user able to see the same title of specific product.</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1738,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1742,6 +1778,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,7 +1884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1880,18 +1922,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1899,9 +1929,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1919,6 +1946,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1933,6 +1975,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2751,470 +2796,477 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="K24" sqref="K24:V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
     </row>
     <row r="5" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
     </row>
     <row r="6" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
     </row>
     <row r="8" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
     </row>
     <row r="9" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
     </row>
     <row r="10" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
     </row>
     <row r="11" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="18"/>
-      <c r="K14" s="19" t="s">
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="K14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="21"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="17"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18"/>
-      <c r="K15" s="22" t="s">
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
+      <c r="K15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="21"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="17"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18"/>
-      <c r="K16" s="23" t="s">
+      <c r="H16" s="24"/>
+      <c r="I16" s="25"/>
+      <c r="K16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="25"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="20"/>
     </row>
     <row r="19" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-      <c r="K19" s="19" t="s">
+      <c r="H19" s="24"/>
+      <c r="I19" s="25"/>
+      <c r="K19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="21"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="17"/>
     </row>
     <row r="20" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="K20" s="19" t="s">
+      <c r="H20" s="24"/>
+      <c r="I20" s="25"/>
+      <c r="K20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="21"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="17"/>
     </row>
     <row r="21" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="18"/>
-      <c r="K21" s="23" t="s">
+      <c r="H21" s="24"/>
+      <c r="I21" s="25"/>
+      <c r="K21" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="25"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="20"/>
     </row>
     <row r="24" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="18"/>
-      <c r="K24" s="26">
+      <c r="H24" s="24"/>
+      <c r="I24" s="25"/>
+      <c r="K24" s="21">
         <v>45433</v>
       </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
+      <c r="V24" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:Z11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="K14:V14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="K15:V15"/>
+    <mergeCell ref="K16:V16"/>
     <mergeCell ref="K19:V19"/>
     <mergeCell ref="K20:V20"/>
     <mergeCell ref="K21:V21"/>
@@ -3223,13 +3275,6 @@
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A1:Z11"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="K14:V14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K15:V15"/>
-    <mergeCell ref="K16:V16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K15" r:id="rId1" xr:uid="{B39E7FA7-0077-4592-BE7E-C6FE950055E9}"/>
@@ -3243,7 +3288,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3403,10 +3448,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C1E1C6-748F-4782-83CA-6948B67C52D3}">
-  <dimension ref="A1:H125"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,7 +3505,7 @@
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="33">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3484,7 +3529,7 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="33">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -3508,7 +3553,7 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="33">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3532,7 +3577,7 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="33">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -3556,7 +3601,7 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="33">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -3580,7 +3625,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="33">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -3604,7 +3649,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="33">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -3628,7 +3673,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="33">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -3786,7 +3831,7 @@
       <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="33">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -3812,7 +3857,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="33">
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -3838,7 +3883,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="33">
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -3864,7 +3909,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="33">
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -4004,7 +4049,7 @@
       <c r="H25" s="30"/>
     </row>
     <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="33">
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -4028,7 +4073,7 @@
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="33">
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -4051,33 +4096,43 @@
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
-    </row>
-    <row r="29" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>207</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>209</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>59</v>
+        <v>211</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>23</v>
@@ -4087,109 +4142,101 @@
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>25</v>
-      </c>
-      <c r="B30" s="4" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
+    </row>
+    <row r="31" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A31" s="33">
+        <v>26</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
+        <v>27</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>25</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>26</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>28</v>
+      <c r="A34" s="33">
+        <v>29</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>88</v>
@@ -4204,14 +4251,14 @@
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>29</v>
+      <c r="A35" s="33">
+        <v>30</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>88</v>
@@ -4226,17 +4273,17 @@
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>30</v>
+      <c r="A36" s="33">
+        <v>31</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>87</v>
@@ -4248,17 +4295,17 @@
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>31</v>
+      <c r="A37" s="33">
+        <v>32</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>87</v>
@@ -4270,17 +4317,17 @@
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>32</v>
+      <c r="A38" s="33">
+        <v>33</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>87</v>
@@ -4291,21 +4338,21 @@
       <c r="G38" s="5"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>33</v>
+    <row r="39" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A39" s="33">
+        <v>34</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>203</v>
+        <v>92</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>23</v>
@@ -4313,21 +4360,21 @@
       <c r="G39" s="5"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>34</v>
+    <row r="40" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A40" s="33">
+        <v>35</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>23</v>
@@ -4335,21 +4382,21 @@
       <c r="G40" s="5"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" ht="195" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>35</v>
+    <row r="41" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A41" s="33">
+        <v>36</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>23</v>
@@ -4357,125 +4404,125 @@
       <c r="G41" s="5"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>36</v>
+    <row r="42" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A42" s="33">
+        <v>37</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A43" s="33">
+        <v>38</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>39</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F44" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>37</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>40</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F45" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G45" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="45" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>38</v>
-      </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="33">
+        <v>41</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>39</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>40</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>23</v>
@@ -4483,51 +4530,75 @@
       <c r="G47" s="5"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>41</v>
+    <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="33">
+        <v>42</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33">
+        <v>43</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="3"/>
+    <row r="50" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="33">
+        <v>44</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -5279,15 +5350,35 @@
       <c r="G125" s="5"/>
       <c r="H125" s="3"/>
     </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="3"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A30:H30"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G45:G125 G4:G15 G17:G24 G26:G27 G29:G43" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G47:G127 G4:G15 G17:G24 G31:G45 G26:G29" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
       <formula1>"A- High, B - Medium, C - Low, None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3" xr:uid="{9E7A5853-1C00-445C-9290-798981E423AE}">
@@ -5302,7 +5393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9830D0D6-2CFD-44B9-BA8F-41E0191DF7BC}">
   <dimension ref="A1:B591"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L135" sqref="L135"/>
     </sheetView>
   </sheetViews>

</xml_diff>